<commit_message>
This is my second commit. Dataprovider is modified with hashmap as argument
</commit_message>
<xml_diff>
--- a/excel/testdataFordataproviderDemoTest.xlsx
+++ b/excel/testdataFordataproviderDemoTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ExcelDataDrivenFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\eclipse-workspace6\SeleniumTraining\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595AC0A8-FECF-4AC9-BA82-B76599F678AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2237B0E6-4532-40F4-AA73-39758225A895}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{E9633B21-E51B-4E50-A84E-1F14B21E2374}"/>
   </bookViews>

</xml_diff>